<commit_message>
updated for data preprocessing
</commit_message>
<xml_diff>
--- a/2021_legrest/data/train/data_config.xlsx
+++ b/2021_legrest/data/train/data_config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -41,6 +41,18 @@
   </si>
   <si>
     <t xml:space="preserve">bestfit_angle_relax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start_angle_standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end_angle_standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start_angle_relax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end_angle_relax</t>
   </si>
   <si>
     <t xml:space="preserve">fsr_matrix_1d_datafile</t>
@@ -164,17 +176,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="topLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="20.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="28.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="28.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -208,6 +231,18 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -231,47 +266,18 @@
       <c r="G2" s="0" t="n">
         <v>811</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>12</v>
+      <c r="L2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>176</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>64</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>1036</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>811</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="N3" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
add converted datasets more
</commit_message>
<xml_diff>
--- a/2021_legrest/data/train/data_config.xlsx
+++ b/2021_legrest/data/train/data_config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -77,6 +77,96 @@
   </si>
   <si>
     <t xml:space="preserve">data_01m.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 10:45:51.782</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 10:45:57.515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 10:46:18.932</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 10:46:25.024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210310T104529-1dm.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_02m.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 11:06:35.585</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 11:06:41.334</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 11:07:02.313</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 11:07:08.062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210310T110616-1dm.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_03m.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 13:25:47.914</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 13:25:53.709</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 13:26:15.048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 13:26:21.218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210310T132548-1dm.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_04m.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 15:33:35.481</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 15:33:41.449</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 15:34:02.756</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 15:34:08.864</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210310T153307-1dm.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_05m.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 15:49:33.587</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 15:49:39.508</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 15:50:00.284</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-10 15:50:06.314</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210310T154900-1dm.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_06m.csv</t>
   </si>
 </sst>
 </file>
@@ -87,7 +177,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Noto Sans CJK KR"/>
@@ -108,11 +198,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Noto Sans CJK KR"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -157,7 +242,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -172,14 +257,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -203,13 +280,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J33" activeCellId="0" sqref="J33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.88"/>
@@ -218,9 +295,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="22.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="23.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.04"/>
@@ -252,13 +329,13 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
@@ -290,27 +367,229 @@
       <c r="G2" s="0" t="n">
         <v>811</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="L2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M3" s="6"/>
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>177</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>784</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>689</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>163</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>809</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>646</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>167</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>738</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>712</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1016</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>768</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>173</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>805</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>638</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>